<commit_message>
Rename ModelTrainingAndValidation folder - model validation is now a separate folder
</commit_message>
<xml_diff>
--- a/DataPreprocessing/DatasetDescriptiveStats.xlsx
+++ b/DataPreprocessing/DatasetDescriptiveStats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\larkinan\Documents\GreenTweet_MultipleBiLSTM\DataPreprocessing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3F1AF651-A739-46C8-8538-DD449CE6E28B}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD09DCB5-3F6C-4614-8311-EF3F3B8B96FB}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="51600" windowHeight="19005" xr2:uid="{630E1060-03AD-41CB-835C-B2D3F30288F4}"/>
   </bookViews>
@@ -369,12 +369,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
@@ -405,12 +399,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -420,6 +408,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -738,7 +738,7 @@
   <dimension ref="A1:N63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -747,23 +747,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
-      <c r="A1" s="48"/>
-      <c r="B1" s="22" t="s">
+      <c r="A1" s="56"/>
+      <c r="B1" s="54" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="22" t="s">
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="23"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="55"/>
     </row>
     <row r="2" spans="1:14">
-      <c r="A2" s="49"/>
+      <c r="A2" s="57"/>
       <c r="B2" s="15" t="s">
         <v>0</v>
       </c>
@@ -776,7 +776,7 @@
       <c r="E2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="40"/>
+      <c r="F2" s="38"/>
       <c r="G2" s="15" t="s">
         <v>0</v>
       </c>
@@ -806,7 +806,7 @@
       <c r="E3" s="3">
         <v>42532</v>
       </c>
-      <c r="F3" s="40"/>
+      <c r="F3" s="38"/>
       <c r="G3" s="3">
         <f>62963-B3</f>
         <v>26309</v>
@@ -840,11 +840,11 @@
         <f>(D3/5000)*100</f>
         <v>59.62</v>
       </c>
-      <c r="E4" s="30">
+      <c r="E4" s="28">
         <f>(E3/72963)*100</f>
         <v>58.292559242355715</v>
       </c>
-      <c r="F4" s="41"/>
+      <c r="F4" s="39"/>
       <c r="G4" s="15">
         <f>100-B4</f>
         <v>41.784857773613069</v>
@@ -865,35 +865,35 @@
     <row r="5" spans="1:14">
       <c r="A5" s="8"/>
       <c r="E5" s="1"/>
-      <c r="F5" s="41"/>
-      <c r="J5" s="36"/>
+      <c r="F5" s="39"/>
+      <c r="J5" s="34"/>
     </row>
     <row r="6" spans="1:14">
-      <c r="A6" s="50" t="s">
+      <c r="A6" s="46" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="16"/>
       <c r="C6" s="16"/>
       <c r="D6" s="16"/>
       <c r="E6" s="16"/>
-      <c r="F6" s="42"/>
+      <c r="F6" s="40"/>
       <c r="G6" s="16"/>
       <c r="H6" s="16"/>
       <c r="I6" s="16"/>
       <c r="J6" s="18"/>
     </row>
     <row r="7" spans="1:14">
-      <c r="A7" s="51" t="s">
+      <c r="A7" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="40"/>
-      <c r="J7" s="36"/>
+      <c r="F7" s="38"/>
+      <c r="J7" s="34"/>
     </row>
     <row r="8" spans="1:14">
-      <c r="A8" s="26" t="s">
+      <c r="A8" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="28">
+      <c r="B8" s="26">
         <f>(2550/B3)*100</f>
         <v>6.956948764118513</v>
       </c>
@@ -906,7 +906,7 @@
       <c r="E8" s="3">
         <v>6.87</v>
       </c>
-      <c r="F8" s="40"/>
+      <c r="F8" s="38"/>
       <c r="G8" s="2">
         <v>2.35</v>
       </c>
@@ -921,7 +921,7 @@
       </c>
     </row>
     <row r="9" spans="1:14">
-      <c r="A9" s="27" t="s">
+      <c r="A9" s="25" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="10">
@@ -937,11 +937,11 @@
       <c r="E9" s="6">
         <v>6.35</v>
       </c>
-      <c r="F9" s="40"/>
+      <c r="F9" s="38"/>
       <c r="G9" s="5">
         <v>0.94</v>
       </c>
-      <c r="H9" s="32">
+      <c r="H9" s="30">
         <v>1.1399999999999999</v>
       </c>
       <c r="I9" s="6">
@@ -952,7 +952,7 @@
       </c>
     </row>
     <row r="10" spans="1:14">
-      <c r="A10" s="27" t="s">
+      <c r="A10" s="25" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="10">
@@ -968,11 +968,11 @@
       <c r="E10" s="6">
         <v>8.8800000000000008</v>
       </c>
-      <c r="F10" s="40"/>
+      <c r="F10" s="38"/>
       <c r="G10" s="5">
         <v>0.65</v>
       </c>
-      <c r="H10" s="32">
+      <c r="H10" s="30">
         <v>0.86</v>
       </c>
       <c r="I10" s="6">
@@ -983,7 +983,7 @@
       </c>
     </row>
     <row r="11" spans="1:14">
-      <c r="A11" s="27" t="s">
+      <c r="A11" s="25" t="s">
         <v>8</v>
       </c>
       <c r="B11" s="10">
@@ -999,14 +999,14 @@
       <c r="E11" s="6">
         <v>13.08</v>
       </c>
-      <c r="F11" s="40"/>
+      <c r="F11" s="38"/>
       <c r="G11" s="5">
         <v>5.23</v>
       </c>
-      <c r="H11" s="32">
+      <c r="H11" s="30">
         <v>4.5199999999999996</v>
       </c>
-      <c r="I11" s="32">
+      <c r="I11" s="30">
         <v>5.05</v>
       </c>
       <c r="J11" s="8">
@@ -1014,7 +1014,7 @@
       </c>
     </row>
     <row r="12" spans="1:14">
-      <c r="A12" s="27" t="s">
+      <c r="A12" s="25" t="s">
         <v>9</v>
       </c>
       <c r="B12" s="10">
@@ -1030,23 +1030,23 @@
       <c r="E12" s="6">
         <v>1.37</v>
       </c>
-      <c r="F12" s="40"/>
+      <c r="F12" s="38"/>
       <c r="G12" s="5">
         <v>0.35</v>
       </c>
-      <c r="H12" s="32">
+      <c r="H12" s="30">
         <v>0.43</v>
       </c>
-      <c r="I12" s="32">
+      <c r="I12" s="30">
         <v>0.5</v>
       </c>
       <c r="J12" s="8">
         <v>0.36</v>
       </c>
-      <c r="N12" s="57"/>
+      <c r="N12" s="53"/>
     </row>
     <row r="13" spans="1:14">
-      <c r="A13" s="27" t="s">
+      <c r="A13" s="25" t="s">
         <v>10</v>
       </c>
       <c r="B13" s="10">
@@ -1062,84 +1062,84 @@
       <c r="E13" s="6">
         <v>1.07</v>
       </c>
-      <c r="F13" s="40"/>
+      <c r="F13" s="38"/>
       <c r="G13" s="5">
         <v>0.2</v>
       </c>
-      <c r="H13" s="32">
+      <c r="H13" s="30">
         <v>0.38</v>
       </c>
-      <c r="I13" s="32">
+      <c r="I13" s="30">
         <v>0.01</v>
       </c>
       <c r="J13" s="8">
         <v>0.2</v>
       </c>
-      <c r="N13" s="57"/>
+      <c r="N13" s="53"/>
     </row>
     <row r="14" spans="1:14">
-      <c r="A14" s="47"/>
-      <c r="B14" s="46"/>
-      <c r="C14" s="46"/>
-      <c r="D14" s="46"/>
-      <c r="E14" s="46"/>
-      <c r="F14" s="42"/>
-      <c r="G14" s="45"/>
-      <c r="H14" s="46"/>
-      <c r="I14" s="46"/>
-      <c r="J14" s="36"/>
-      <c r="N14" s="57"/>
+      <c r="A14" s="45"/>
+      <c r="B14" s="44"/>
+      <c r="C14" s="44"/>
+      <c r="D14" s="44"/>
+      <c r="E14" s="44"/>
+      <c r="F14" s="40"/>
+      <c r="G14" s="43"/>
+      <c r="H14" s="44"/>
+      <c r="I14" s="44"/>
+      <c r="J14" s="34"/>
+      <c r="N14" s="53"/>
     </row>
     <row r="15" spans="1:14">
-      <c r="A15" s="51" t="s">
+      <c r="A15" s="47" t="s">
         <v>20</v>
       </c>
-      <c r="F15" s="40"/>
+      <c r="F15" s="38"/>
       <c r="G15" s="12"/>
       <c r="J15" s="14"/>
-      <c r="N15" s="57"/>
+      <c r="N15" s="53"/>
     </row>
     <row r="16" spans="1:14">
       <c r="A16" s="19">
         <v>1</v>
       </c>
-      <c r="B16" s="28">
+      <c r="B16" s="26">
         <f>(24163/36654)*100</f>
         <v>65.921863916625739</v>
       </c>
-      <c r="C16" s="28">
+      <c r="C16" s="26">
         <f>(1878/2897)*100</f>
         <v>64.825681739730754</v>
       </c>
-      <c r="D16" s="28">
+      <c r="D16" s="26">
         <f>(1997/2981)*100</f>
         <v>66.990942636699089</v>
       </c>
-      <c r="E16" s="28">
+      <c r="E16" s="26">
         <f>(28038/E3)*100</f>
         <v>65.922129220351735</v>
       </c>
-      <c r="F16" s="41"/>
-      <c r="G16" s="24">
+      <c r="F16" s="39"/>
+      <c r="G16" s="22">
         <f>(2376/G3)*100</f>
         <v>9.0311300315481393</v>
       </c>
-      <c r="H16" s="28">
+      <c r="H16" s="26">
         <f>(187/H3)*100</f>
         <v>8.8920589633856384</v>
       </c>
-      <c r="I16" s="28">
+      <c r="I16" s="26">
         <f>(173/I3)*100</f>
         <v>8.5685983159980186</v>
       </c>
-      <c r="J16" s="29">
+      <c r="J16" s="27">
         <f>(2736/J3)*100</f>
         <v>8.9908317176563379</v>
       </c>
-      <c r="N16" s="57"/>
+      <c r="N16" s="53"/>
     </row>
     <row r="17" spans="1:14">
-      <c r="A17" s="31">
+      <c r="A17" s="29">
         <v>2</v>
       </c>
       <c r="B17" s="10">
@@ -1158,7 +1158,7 @@
         <f>(13029/E3)*100</f>
         <v>30.633405435907079</v>
       </c>
-      <c r="F17" s="41"/>
+      <c r="F17" s="39"/>
       <c r="G17" s="9">
         <f>(89/G3)*100</f>
         <v>0.33828727811775439</v>
@@ -1175,10 +1175,10 @@
         <f>(108/J3)*100</f>
         <v>0.35490125201275019</v>
       </c>
-      <c r="N17" s="57"/>
+      <c r="N17" s="53"/>
     </row>
     <row r="18" spans="1:14">
-      <c r="A18" s="31">
+      <c r="A18" s="29">
         <v>3</v>
       </c>
       <c r="B18" s="10">
@@ -1197,7 +1197,7 @@
         <f>(1426/E3)*100</f>
         <v>3.3527696793002915</v>
       </c>
-      <c r="F18" s="41"/>
+      <c r="F18" s="39"/>
       <c r="G18" s="9" t="s">
         <v>12</v>
       </c>
@@ -1210,10 +1210,10 @@
       <c r="J18" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="N18" s="57"/>
+      <c r="N18" s="53"/>
     </row>
     <row r="19" spans="1:14">
-      <c r="A19" s="31">
+      <c r="A19" s="29">
         <v>4</v>
       </c>
       <c r="B19" s="10">
@@ -1232,7 +1232,7 @@
         <f>(36/E3)*100</f>
         <v>8.4642151791592221E-2</v>
       </c>
-      <c r="F19" s="41"/>
+      <c r="F19" s="39"/>
       <c r="G19" s="9">
         <v>0</v>
       </c>
@@ -1245,10 +1245,10 @@
       <c r="J19" s="7">
         <v>0</v>
       </c>
-      <c r="N19" s="57"/>
+      <c r="N19" s="53"/>
     </row>
     <row r="20" spans="1:14">
-      <c r="A20" s="31">
+      <c r="A20" s="29">
         <v>5</v>
       </c>
       <c r="B20" s="10" t="s">
@@ -1263,7 +1263,7 @@
       <c r="E20" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="F20" s="41"/>
+      <c r="F20" s="39"/>
       <c r="G20" s="9">
         <v>0</v>
       </c>
@@ -1278,7 +1278,7 @@
       </c>
     </row>
     <row r="21" spans="1:14">
-      <c r="A21" s="31">
+      <c r="A21" s="29">
         <v>6</v>
       </c>
       <c r="B21" s="10">
@@ -1293,7 +1293,7 @@
       <c r="E21" s="10">
         <v>0</v>
       </c>
-      <c r="F21" s="41"/>
+      <c r="F21" s="39"/>
       <c r="G21" s="9">
         <v>0</v>
       </c>
@@ -1311,26 +1311,26 @@
       <c r="A22" s="20">
         <v>7</v>
       </c>
-      <c r="B22" s="30" t="s">
+      <c r="B22" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="C22" s="30">
-        <v>0</v>
-      </c>
-      <c r="D22" s="30">
-        <v>0</v>
-      </c>
-      <c r="E22" s="30" t="s">
+      <c r="C22" s="28">
+        <v>0</v>
+      </c>
+      <c r="D22" s="28">
+        <v>0</v>
+      </c>
+      <c r="E22" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="F22" s="41"/>
-      <c r="G22" s="25">
-        <v>0</v>
-      </c>
-      <c r="H22" s="30">
-        <v>0</v>
-      </c>
-      <c r="I22" s="30">
+      <c r="F22" s="39"/>
+      <c r="G22" s="23">
+        <v>0</v>
+      </c>
+      <c r="H22" s="28">
+        <v>0</v>
+      </c>
+      <c r="I22" s="28">
         <v>0</v>
       </c>
       <c r="J22" s="21">
@@ -1343,39 +1343,39 @@
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
-      <c r="F23" s="41"/>
-      <c r="G23" s="53"/>
+      <c r="F23" s="39"/>
+      <c r="G23" s="49"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
-      <c r="J23" s="37"/>
+      <c r="J23" s="35"/>
     </row>
     <row r="24" spans="1:14">
-      <c r="A24" s="50" t="s">
+      <c r="A24" s="46" t="s">
         <v>16</v>
       </c>
       <c r="B24" s="16"/>
       <c r="C24" s="16"/>
       <c r="D24" s="16"/>
       <c r="E24" s="17"/>
-      <c r="F24" s="43"/>
-      <c r="G24" s="54"/>
+      <c r="F24" s="41"/>
+      <c r="G24" s="50"/>
       <c r="H24" s="16"/>
       <c r="I24" s="16"/>
       <c r="J24" s="18"/>
     </row>
     <row r="25" spans="1:14">
-      <c r="A25" s="52" t="s">
+      <c r="A25" s="48" t="s">
         <v>24</v>
       </c>
-      <c r="B25" s="32"/>
-      <c r="C25" s="32"/>
-      <c r="D25" s="32"/>
-      <c r="E25" s="33"/>
-      <c r="F25" s="41"/>
-      <c r="G25" s="55"/>
-      <c r="H25" s="32"/>
-      <c r="I25" s="32"/>
-      <c r="J25" s="34"/>
+      <c r="B25" s="30"/>
+      <c r="C25" s="30"/>
+      <c r="D25" s="30"/>
+      <c r="E25" s="31"/>
+      <c r="F25" s="39"/>
+      <c r="G25" s="51"/>
+      <c r="H25" s="30"/>
+      <c r="I25" s="30"/>
+      <c r="J25" s="32"/>
     </row>
     <row r="26" spans="1:14">
       <c r="A26" s="19">
@@ -1393,7 +1393,7 @@
       <c r="E26" s="3">
         <v>1</v>
       </c>
-      <c r="F26" s="40"/>
+      <c r="F26" s="38"/>
       <c r="G26" s="2">
         <v>1</v>
       </c>
@@ -1408,7 +1408,7 @@
       </c>
     </row>
     <row r="27" spans="1:14">
-      <c r="A27" s="31">
+      <c r="A27" s="29">
         <v>24</v>
       </c>
       <c r="B27" s="6">
@@ -1423,11 +1423,11 @@
       <c r="E27" s="6">
         <v>2</v>
       </c>
-      <c r="F27" s="40"/>
+      <c r="F27" s="38"/>
       <c r="G27" s="5">
         <v>2</v>
       </c>
-      <c r="H27" s="32">
+      <c r="H27" s="30">
         <v>2</v>
       </c>
       <c r="I27" s="6">
@@ -1438,7 +1438,7 @@
       </c>
     </row>
     <row r="28" spans="1:14">
-      <c r="A28" s="31">
+      <c r="A28" s="29">
         <v>50</v>
       </c>
       <c r="B28" s="6">
@@ -1453,11 +1453,11 @@
       <c r="E28" s="6">
         <v>4</v>
       </c>
-      <c r="F28" s="40"/>
+      <c r="F28" s="38"/>
       <c r="G28" s="5">
         <v>4</v>
       </c>
-      <c r="H28" s="32">
+      <c r="H28" s="30">
         <v>4</v>
       </c>
       <c r="I28" s="6">
@@ -1468,7 +1468,7 @@
       </c>
     </row>
     <row r="29" spans="1:14">
-      <c r="A29" s="31">
+      <c r="A29" s="29">
         <v>75</v>
       </c>
       <c r="B29" s="6">
@@ -1483,14 +1483,14 @@
       <c r="E29" s="6">
         <v>6</v>
       </c>
-      <c r="F29" s="40"/>
+      <c r="F29" s="38"/>
       <c r="G29" s="5">
         <v>6</v>
       </c>
-      <c r="H29" s="32">
+      <c r="H29" s="30">
         <v>6</v>
       </c>
-      <c r="I29" s="32">
+      <c r="I29" s="30">
         <v>6</v>
       </c>
       <c r="J29" s="8">
@@ -1513,7 +1513,7 @@
       <c r="E30" s="15">
         <v>12</v>
       </c>
-      <c r="F30" s="40"/>
+      <c r="F30" s="38"/>
       <c r="G30" s="12">
         <v>15</v>
       </c>
@@ -1528,12 +1528,12 @@
       </c>
     </row>
     <row r="31" spans="1:14">
-      <c r="A31" s="31"/>
+      <c r="A31" s="29"/>
       <c r="B31" s="6"/>
       <c r="C31" s="6"/>
       <c r="D31" s="6"/>
       <c r="E31" s="6"/>
-      <c r="F31" s="40"/>
+      <c r="F31" s="38"/>
       <c r="G31" s="5"/>
       <c r="H31" s="6"/>
       <c r="I31" s="6"/>
@@ -1543,42 +1543,42 @@
       <c r="A32" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="B32" s="28">
+      <c r="B32" s="26">
         <f>(3671/B3)*100</f>
         <v>10.015278005129044</v>
       </c>
-      <c r="C32" s="28">
+      <c r="C32" s="26">
         <f>(297/2897)*100</f>
         <v>10.251984811874353</v>
       </c>
-      <c r="D32" s="28">
+      <c r="D32" s="26">
         <f>(347/2981)*100</f>
         <v>11.640389131164039</v>
       </c>
-      <c r="E32" s="28">
+      <c r="E32" s="26">
         <f>(4315/E3)*100</f>
         <v>10.145302360575567</v>
       </c>
-      <c r="F32" s="41"/>
-      <c r="G32" s="24">
+      <c r="F32" s="39"/>
+      <c r="G32" s="22">
         <f>(1559/G3)*100</f>
         <v>5.9257288380402144</v>
       </c>
-      <c r="H32" s="28">
+      <c r="H32" s="26">
         <f>(128/H3)*100</f>
         <v>6.0865430337612931</v>
       </c>
-      <c r="I32" s="28">
+      <c r="I32" s="26">
         <f>(127/I3)*100</f>
         <v>6.2902426944031697</v>
       </c>
-      <c r="J32" s="29">
+      <c r="J32" s="27">
         <f>(1814/J3)*100</f>
         <v>5.9610265847326742</v>
       </c>
     </row>
     <row r="33" spans="1:10">
-      <c r="A33" s="31" t="s">
+      <c r="A33" s="29" t="s">
         <v>22</v>
       </c>
       <c r="B33" s="6">
@@ -1593,14 +1593,14 @@
       <c r="E33" s="6">
         <v>44</v>
       </c>
-      <c r="F33" s="40"/>
+      <c r="F33" s="38"/>
       <c r="G33" s="5">
         <v>57</v>
       </c>
-      <c r="H33" s="32">
+      <c r="H33" s="30">
         <v>45</v>
       </c>
-      <c r="I33" s="32">
+      <c r="I33" s="30">
         <v>28</v>
       </c>
       <c r="J33" s="8">
@@ -1608,7 +1608,7 @@
       </c>
     </row>
     <row r="34" spans="1:10">
-      <c r="A34" s="31" t="s">
+      <c r="A34" s="29" t="s">
         <v>23</v>
       </c>
       <c r="B34" s="6">
@@ -1623,14 +1623,14 @@
       <c r="E34" s="6">
         <v>0</v>
       </c>
-      <c r="F34" s="40"/>
+      <c r="F34" s="38"/>
       <c r="G34" s="5">
         <v>0</v>
       </c>
-      <c r="H34" s="32">
-        <v>0</v>
-      </c>
-      <c r="I34" s="32">
+      <c r="H34" s="30">
+        <v>0</v>
+      </c>
+      <c r="I34" s="30">
         <v>0</v>
       </c>
       <c r="J34" s="8">
@@ -1638,7 +1638,7 @@
       </c>
     </row>
     <row r="35" spans="1:10">
-      <c r="A35" s="31" t="s">
+      <c r="A35" s="29" t="s">
         <v>28</v>
       </c>
       <c r="B35" s="6">
@@ -1653,11 +1653,11 @@
       <c r="E35" s="6">
         <v>4.74</v>
       </c>
-      <c r="F35" s="40"/>
+      <c r="F35" s="38"/>
       <c r="G35" s="5">
         <v>5.18</v>
       </c>
-      <c r="H35" s="32">
+      <c r="H35" s="30">
         <v>4.9800000000000004</v>
       </c>
       <c r="I35" s="6">
@@ -1683,7 +1683,7 @@
       <c r="E36" s="15">
         <v>4.1100000000000003</v>
       </c>
-      <c r="F36" s="44"/>
+      <c r="F36" s="42"/>
       <c r="G36" s="12">
         <v>5.3</v>
       </c>
@@ -1699,37 +1699,37 @@
     </row>
     <row r="37" spans="1:10">
       <c r="A37" s="8"/>
-      <c r="F37" s="40"/>
-      <c r="G37" s="45"/>
-      <c r="J37" s="36"/>
+      <c r="F37" s="38"/>
+      <c r="G37" s="43"/>
+      <c r="J37" s="34"/>
     </row>
     <row r="38" spans="1:10">
-      <c r="A38" s="50" t="s">
+      <c r="A38" s="46" t="s">
         <v>17</v>
       </c>
       <c r="B38" s="16"/>
       <c r="C38" s="16"/>
       <c r="D38" s="16"/>
       <c r="E38" s="17"/>
-      <c r="F38" s="43"/>
-      <c r="G38" s="54"/>
+      <c r="F38" s="41"/>
+      <c r="G38" s="50"/>
       <c r="H38" s="16"/>
       <c r="I38" s="16"/>
       <c r="J38" s="18"/>
     </row>
     <row r="39" spans="1:10">
-      <c r="A39" s="52" t="s">
+      <c r="A39" s="48" t="s">
         <v>24</v>
       </c>
-      <c r="B39" s="32"/>
-      <c r="C39" s="32"/>
-      <c r="D39" s="32"/>
-      <c r="E39" s="33"/>
-      <c r="F39" s="41"/>
-      <c r="G39" s="56"/>
-      <c r="H39" s="32"/>
-      <c r="I39" s="32"/>
-      <c r="J39" s="38"/>
+      <c r="B39" s="30"/>
+      <c r="C39" s="30"/>
+      <c r="D39" s="30"/>
+      <c r="E39" s="31"/>
+      <c r="F39" s="39"/>
+      <c r="G39" s="52"/>
+      <c r="H39" s="30"/>
+      <c r="I39" s="30"/>
+      <c r="J39" s="36"/>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="19">
@@ -1747,7 +1747,7 @@
       <c r="E40" s="3">
         <v>1</v>
       </c>
-      <c r="F40" s="40"/>
+      <c r="F40" s="38"/>
       <c r="G40" s="2">
         <v>1</v>
       </c>
@@ -1762,7 +1762,7 @@
       </c>
     </row>
     <row r="41" spans="1:10">
-      <c r="A41" s="31">
+      <c r="A41" s="29">
         <v>25</v>
       </c>
       <c r="B41" s="6">
@@ -1777,11 +1777,11 @@
       <c r="E41" s="6">
         <v>2</v>
       </c>
-      <c r="F41" s="40"/>
+      <c r="F41" s="38"/>
       <c r="G41" s="5">
         <v>2</v>
       </c>
-      <c r="H41" s="32">
+      <c r="H41" s="30">
         <v>2</v>
       </c>
       <c r="I41" s="6">
@@ -1792,7 +1792,7 @@
       </c>
     </row>
     <row r="42" spans="1:10">
-      <c r="A42" s="31">
+      <c r="A42" s="29">
         <v>50</v>
       </c>
       <c r="B42" s="6">
@@ -1807,11 +1807,11 @@
       <c r="E42" s="6">
         <v>3</v>
       </c>
-      <c r="F42" s="40"/>
+      <c r="F42" s="38"/>
       <c r="G42" s="5">
         <v>3</v>
       </c>
-      <c r="H42" s="32">
+      <c r="H42" s="30">
         <v>3</v>
       </c>
       <c r="I42" s="6">
@@ -1822,7 +1822,7 @@
       </c>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="31">
+      <c r="A43" s="29">
         <v>75</v>
       </c>
       <c r="B43" s="6">
@@ -1837,14 +1837,14 @@
       <c r="E43" s="6">
         <v>6</v>
       </c>
-      <c r="F43" s="40"/>
+      <c r="F43" s="38"/>
       <c r="G43" s="5">
         <v>4</v>
       </c>
-      <c r="H43" s="32">
+      <c r="H43" s="30">
         <v>4</v>
       </c>
-      <c r="I43" s="32">
+      <c r="I43" s="30">
         <v>4</v>
       </c>
       <c r="J43" s="8">
@@ -1867,7 +1867,7 @@
       <c r="E44" s="15">
         <v>10</v>
       </c>
-      <c r="F44" s="40"/>
+      <c r="F44" s="38"/>
       <c r="G44" s="12">
         <v>8</v>
       </c>
@@ -1883,50 +1883,50 @@
     </row>
     <row r="45" spans="1:10">
       <c r="A45" s="8"/>
-      <c r="F45" s="40"/>
-      <c r="G45" s="45"/>
-      <c r="J45" s="36"/>
+      <c r="F45" s="38"/>
+      <c r="G45" s="43"/>
+      <c r="J45" s="34"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="B46" s="28">
+      <c r="B46" s="26">
         <f>(8767/B3)*100</f>
         <v>23.918262672559614</v>
       </c>
-      <c r="C46" s="28">
+      <c r="C46" s="26">
         <f>(701/28997)*1000</f>
         <v>24.174914646342724</v>
       </c>
-      <c r="D46" s="28">
+      <c r="D46" s="26">
         <f>(742/2981)*100</f>
         <v>24.890976182489098</v>
       </c>
-      <c r="E46" s="28">
+      <c r="E46" s="26">
         <f>(10210/E3)*100</f>
         <v>24.005454716448789</v>
       </c>
-      <c r="F46" s="41"/>
-      <c r="G46" s="24">
+      <c r="F46" s="39"/>
+      <c r="G46" s="22">
         <f>(4767/G3)*100</f>
         <v>18.119274772891405</v>
       </c>
-      <c r="H46" s="28">
+      <c r="H46" s="26">
         <f>(393/H3)*100</f>
         <v>18.687589158345222</v>
       </c>
-      <c r="I46" s="28">
+      <c r="I46" s="26">
         <f>(342/I3)*100</f>
         <v>16.939078751857355</v>
       </c>
-      <c r="J46" s="29">
+      <c r="J46" s="27">
         <f>(5502/J3)*100</f>
         <v>18.08024711642733</v>
       </c>
     </row>
     <row r="47" spans="1:10">
-      <c r="A47" s="31" t="s">
+      <c r="A47" s="29" t="s">
         <v>22</v>
       </c>
       <c r="B47" s="6">
@@ -1941,14 +1941,14 @@
       <c r="E47" s="6">
         <v>26</v>
       </c>
-      <c r="F47" s="40"/>
+      <c r="F47" s="38"/>
       <c r="G47" s="5">
         <v>16</v>
       </c>
-      <c r="H47" s="32">
+      <c r="H47" s="30">
         <v>14</v>
       </c>
-      <c r="I47" s="32">
+      <c r="I47" s="30">
         <v>16</v>
       </c>
       <c r="J47" s="8">
@@ -1956,7 +1956,7 @@
       </c>
     </row>
     <row r="48" spans="1:10">
-      <c r="A48" s="31" t="s">
+      <c r="A48" s="29" t="s">
         <v>23</v>
       </c>
       <c r="B48" s="6">
@@ -1971,14 +1971,14 @@
       <c r="E48" s="6">
         <v>0</v>
       </c>
-      <c r="F48" s="40"/>
+      <c r="F48" s="38"/>
       <c r="G48" s="5">
         <v>0</v>
       </c>
-      <c r="H48" s="32">
-        <v>0</v>
-      </c>
-      <c r="I48" s="32">
+      <c r="H48" s="30">
+        <v>0</v>
+      </c>
+      <c r="I48" s="30">
         <v>0</v>
       </c>
       <c r="J48" s="8">
@@ -1986,7 +1986,7 @@
       </c>
     </row>
     <row r="49" spans="1:10">
-      <c r="A49" s="31" t="s">
+      <c r="A49" s="29" t="s">
         <v>28</v>
       </c>
       <c r="B49" s="6">
@@ -2001,11 +2001,11 @@
       <c r="E49" s="6">
         <v>4.24</v>
       </c>
-      <c r="F49" s="40"/>
+      <c r="F49" s="38"/>
       <c r="G49" s="5">
         <v>3.37</v>
       </c>
-      <c r="H49" s="32">
+      <c r="H49" s="30">
         <v>3.23</v>
       </c>
       <c r="I49" s="6">
@@ -2031,7 +2031,7 @@
       <c r="E50" s="15">
         <v>2.91</v>
       </c>
-      <c r="F50" s="40"/>
+      <c r="F50" s="38"/>
       <c r="G50" s="12">
         <v>2.3199999999999998</v>
       </c>
@@ -2047,31 +2047,31 @@
     </row>
     <row r="51" spans="1:10">
       <c r="A51" s="8"/>
-      <c r="F51" s="40"/>
-      <c r="G51" s="45"/>
-      <c r="J51" s="36"/>
+      <c r="F51" s="38"/>
+      <c r="G51" s="43"/>
+      <c r="J51" s="34"/>
     </row>
     <row r="52" spans="1:10">
-      <c r="A52" s="50" t="s">
+      <c r="A52" s="46" t="s">
         <v>27</v>
       </c>
       <c r="B52" s="16"/>
       <c r="C52" s="16"/>
       <c r="D52" s="16"/>
       <c r="E52" s="17"/>
-      <c r="F52" s="43"/>
-      <c r="G52" s="54"/>
+      <c r="F52" s="41"/>
+      <c r="G52" s="50"/>
       <c r="H52" s="16"/>
       <c r="I52" s="16"/>
       <c r="J52" s="18"/>
     </row>
     <row r="53" spans="1:10">
-      <c r="A53" s="51" t="s">
+      <c r="A53" s="47" t="s">
         <v>24</v>
       </c>
-      <c r="F53" s="40"/>
-      <c r="G53" s="45"/>
-      <c r="J53" s="36"/>
+      <c r="F53" s="38"/>
+      <c r="G53" s="43"/>
+      <c r="J53" s="34"/>
     </row>
     <row r="54" spans="1:10">
       <c r="A54" s="19">
@@ -2080,16 +2080,16 @@
       <c r="B54" s="3">
         <v>8</v>
       </c>
-      <c r="C54" s="35">
+      <c r="C54" s="33">
         <v>8</v>
       </c>
-      <c r="D54" s="35">
+      <c r="D54" s="33">
         <v>8</v>
       </c>
       <c r="E54" s="3">
         <v>8</v>
       </c>
-      <c r="F54" s="40"/>
+      <c r="F54" s="38"/>
       <c r="G54" s="2">
         <v>8</v>
       </c>
@@ -2104,7 +2104,7 @@
       </c>
     </row>
     <row r="55" spans="1:10">
-      <c r="A55" s="31">
+      <c r="A55" s="29">
         <v>25</v>
       </c>
       <c r="B55" s="6">
@@ -2119,7 +2119,7 @@
       <c r="E55" s="6">
         <v>13</v>
       </c>
-      <c r="F55" s="40"/>
+      <c r="F55" s="38"/>
       <c r="G55" s="5">
         <v>14</v>
       </c>
@@ -2134,7 +2134,7 @@
       </c>
     </row>
     <row r="56" spans="1:10">
-      <c r="A56" s="31">
+      <c r="A56" s="29">
         <v>50</v>
       </c>
       <c r="B56" s="6">
@@ -2149,7 +2149,7 @@
       <c r="E56" s="6">
         <v>18</v>
       </c>
-      <c r="F56" s="40"/>
+      <c r="F56" s="38"/>
       <c r="G56" s="5">
         <v>20</v>
       </c>
@@ -2164,7 +2164,7 @@
       </c>
     </row>
     <row r="57" spans="1:10">
-      <c r="A57" s="31">
+      <c r="A57" s="29">
         <v>75</v>
       </c>
       <c r="B57" s="6">
@@ -2179,14 +2179,14 @@
       <c r="E57" s="6">
         <v>23</v>
       </c>
-      <c r="F57" s="40"/>
+      <c r="F57" s="38"/>
       <c r="G57" s="5">
         <v>25</v>
       </c>
-      <c r="H57" s="32">
+      <c r="H57" s="30">
         <v>25</v>
       </c>
-      <c r="I57" s="32">
+      <c r="I57" s="30">
         <v>25</v>
       </c>
       <c r="J57" s="8">
@@ -2209,7 +2209,7 @@
       <c r="E58" s="15">
         <v>30</v>
       </c>
-      <c r="F58" s="40"/>
+      <c r="F58" s="38"/>
       <c r="G58" s="12">
         <v>30</v>
       </c>
@@ -2224,19 +2224,19 @@
       </c>
     </row>
     <row r="59" spans="1:10">
-      <c r="A59" s="36"/>
-      <c r="F59" s="40"/>
-      <c r="G59" s="45"/>
-      <c r="J59" s="36"/>
+      <c r="A59" s="34"/>
+      <c r="F59" s="38"/>
+      <c r="G59" s="43"/>
+      <c r="J59" s="34"/>
     </row>
     <row r="60" spans="1:10">
-      <c r="A60" s="31" t="s">
+      <c r="A60" s="29" t="s">
         <v>22</v>
       </c>
       <c r="B60" s="3">
         <v>113</v>
       </c>
-      <c r="C60" s="35">
+      <c r="C60" s="33">
         <v>54</v>
       </c>
       <c r="D60" s="3">
@@ -2245,7 +2245,7 @@
       <c r="E60" s="3">
         <v>113</v>
       </c>
-      <c r="F60" s="40"/>
+      <c r="F60" s="38"/>
       <c r="G60" s="2">
         <v>94</v>
       </c>
@@ -2260,7 +2260,7 @@
       </c>
     </row>
     <row r="61" spans="1:10">
-      <c r="A61" s="31" t="s">
+      <c r="A61" s="29" t="s">
         <v>23</v>
       </c>
       <c r="B61" s="6">
@@ -2275,14 +2275,14 @@
       <c r="E61" s="6">
         <v>6</v>
       </c>
-      <c r="F61" s="40"/>
+      <c r="F61" s="38"/>
       <c r="G61" s="5">
         <v>6</v>
       </c>
-      <c r="H61" s="32">
+      <c r="H61" s="30">
         <v>6</v>
       </c>
-      <c r="I61" s="32">
+      <c r="I61" s="30">
         <v>6</v>
       </c>
       <c r="J61" s="8">
@@ -2290,7 +2290,7 @@
       </c>
     </row>
     <row r="62" spans="1:10">
-      <c r="A62" s="31" t="s">
+      <c r="A62" s="29" t="s">
         <v>28</v>
       </c>
       <c r="B62" s="6">
@@ -2305,14 +2305,14 @@
       <c r="E62" s="6">
         <v>18.46</v>
       </c>
-      <c r="F62" s="40"/>
+      <c r="F62" s="38"/>
       <c r="G62" s="5">
         <v>19.649999999999999</v>
       </c>
       <c r="H62" s="6">
         <v>19.84</v>
       </c>
-      <c r="I62" s="32">
+      <c r="I62" s="30">
         <v>19.47</v>
       </c>
       <c r="J62" s="8">
@@ -2326,16 +2326,16 @@
       <c r="B63" s="15">
         <v>6.89</v>
       </c>
-      <c r="C63" s="30">
+      <c r="C63" s="28">
         <v>6.97</v>
       </c>
-      <c r="D63" s="30">
+      <c r="D63" s="28">
         <v>6.97</v>
       </c>
       <c r="E63" s="15">
         <v>6.91</v>
       </c>
-      <c r="F63" s="44"/>
+      <c r="F63" s="42"/>
       <c r="G63" s="12">
         <v>7.02</v>
       </c>

</xml_diff>